<commit_message>
update with indexed data
</commit_message>
<xml_diff>
--- a/4-year_public_tuition_INFLATION_ADJUSTED.xlsx
+++ b/4-year_public_tuition_INFLATION_ADJUSTED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/170835/Documents/ALLPROJECTS/updateMillennials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30104C9-B984-2B44-8201-60AA01F36F01}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F8CBC2-51F3-5C45-A9F7-8AEE381AB4B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17880" yWindow="1440" windowWidth="27640" windowHeight="16940" xr2:uid="{8F8FF7DC-2BD5-3649-8C80-A9737280B255}"/>
+    <workbookView xWindow="42200" yWindow="1960" windowWidth="27640" windowHeight="16940" xr2:uid="{8F8FF7DC-2BD5-3649-8C80-A9737280B255}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -72,8 +72,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,7 +391,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB040FC-8FA3-B945-8F18-F7F0662FDF13}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -409,7 +412,7 @@
       <c r="A2">
         <v>1966</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>2279.1864408203728</v>
       </c>
     </row>
@@ -417,7 +420,7 @@
       <c r="A3">
         <v>1967</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2262.3362013549095</v>
       </c>
     </row>
@@ -425,7 +428,7 @@
       <c r="A4">
         <v>1968</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>2233.1295615166455</v>
       </c>
     </row>
@@ -433,7 +436,7 @@
       <c r="A5">
         <v>1969</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2353.8623674779355</v>
       </c>
     </row>
@@ -441,7 +444,7 @@
       <c r="A6">
         <v>1970</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>2459.0149074464048</v>
       </c>
     </row>
@@ -449,7 +452,7 @@
       <c r="A7">
         <v>1971</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>2579.314190008005</v>
       </c>
     </row>
@@ -457,7 +460,7 @@
       <c r="A8">
         <v>1972</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>2913.3482372314747</v>
       </c>
     </row>
@@ -465,7 +468,7 @@
       <c r="A9">
         <v>1973</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>2733.121091585409</v>
       </c>
     </row>
@@ -473,7 +476,7 @@
       <c r="A10">
         <v>1974</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>2454.9092726200761</v>
       </c>
     </row>
@@ -481,7 +484,7 @@
       <c r="A11">
         <v>1975</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>2425.6115905462798</v>
       </c>
     </row>
@@ -489,7 +492,7 @@
       <c r="A12">
         <v>1976</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>2606.544939877876</v>
       </c>
     </row>
@@ -497,7 +500,7 @@
       <c r="A13">
         <v>1977</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>2593.5609681112815</v>
       </c>
     </row>
@@ -505,7 +508,7 @@
       <c r="A14">
         <v>1978</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>2490.9476909993241</v>
       </c>
     </row>
@@ -513,7 +516,7 @@
       <c r="A15">
         <v>1979</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>2357.2982665780501</v>
       </c>
     </row>
@@ -521,7 +524,7 @@
       <c r="A16">
         <v>1980</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>2302.2291152233943</v>
       </c>
     </row>
@@ -529,7 +532,7 @@
       <c r="A17">
         <v>1981</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>2397.994185482592</v>
       </c>
     </row>
@@ -537,7 +540,7 @@
       <c r="A18">
         <v>1982</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>2607.4924646241334</v>
       </c>
     </row>
@@ -545,7 +548,7 @@
       <c r="A19">
         <v>1983</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>2797.9226612396665</v>
       </c>
     </row>
@@ -553,7 +556,7 @@
       <c r="A20">
         <v>1984</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>2880.5711941383902</v>
       </c>
     </row>
@@ -561,7 +564,7 @@
       <c r="A21">
         <v>1985</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>3004.4118006742492</v>
       </c>
     </row>
@@ -569,7 +572,7 @@
       <c r="A22">
         <v>1986</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>3153.4747575970796</v>
       </c>
     </row>
@@ -577,7 +580,7 @@
       <c r="A23">
         <v>1987</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>3292.942157803072</v>
       </c>
     </row>
@@ -585,7 +588,7 @@
       <c r="A24">
         <v>1988</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>3370.3715512753802</v>
       </c>
     </row>
@@ -593,7 +596,7 @@
       <c r="A25">
         <v>1989</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>3477.5922103402781</v>
       </c>
     </row>
@@ -601,7 +604,7 @@
       <c r="A26">
         <v>1990</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>3498.3902289547868</v>
       </c>
     </row>
@@ -609,7 +612,7 @@
       <c r="A27">
         <v>1991</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>3800.4757739229003</v>
       </c>
     </row>
@@ -617,7 +620,7 @@
       <c r="A28">
         <v>1992</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>4089.6327965378346</v>
       </c>
     </row>
@@ -625,7 +628,7 @@
       <c r="A29">
         <v>1993</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>4304.5064639542879</v>
       </c>
     </row>
@@ -633,7 +636,7 @@
       <c r="A30">
         <v>1994</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>4422.3389892202449</v>
       </c>
     </row>
@@ -641,7 +644,7 @@
       <c r="A31">
         <v>1995</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>4573.1936393803153</v>
       </c>
     </row>
@@ -649,7 +652,7 @@
       <c r="A32">
         <v>1996</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>4664.3798155538097</v>
       </c>
     </row>
@@ -657,7 +660,7 @@
       <c r="A33">
         <v>1997</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>4770.2467814736992</v>
       </c>
     </row>
@@ -665,7 +668,7 @@
       <c r="A34">
         <v>1998</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>4868.8395561303005</v>
       </c>
     </row>
@@ -673,7 +676,7 @@
       <c r="A35">
         <v>1999</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>4908.239990243248</v>
       </c>
     </row>
@@ -681,7 +684,7 @@
       <c r="A36">
         <v>2000</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>4960.6564640813176</v>
       </c>
     </row>
@@ -689,7 +692,7 @@
       <c r="A37">
         <v>2001</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>5201.1405599046748</v>
       </c>
     </row>
@@ -697,7 +700,7 @@
       <c r="A38">
         <v>2002</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>5512.9963919924576</v>
       </c>
     </row>
@@ -705,7 +708,7 @@
       <c r="A39">
         <v>2003</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>6115.4696727815272</v>
       </c>
     </row>
@@ -713,7 +716,7 @@
       <c r="A40">
         <v>2004</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>6506.363369577175</v>
       </c>
     </row>
@@ -721,7 +724,7 @@
       <c r="A41">
         <v>2005</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>6672.1511657483343</v>
       </c>
     </row>
@@ -729,7 +732,7 @@
       <c r="A42">
         <v>2006</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>6887.1874042036834</v>
       </c>
     </row>
@@ -737,7 +740,7 @@
       <c r="A43">
         <v>2007</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>6965.6670805155154</v>
       </c>
     </row>
@@ -745,7 +748,7 @@
       <c r="A44">
         <v>2008</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>7295.9453257473551</v>
       </c>
     </row>
@@ -753,7 +756,7 @@
       <c r="A45">
         <v>2009</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>7689.4006256679004</v>
       </c>
     </row>
@@ -761,7 +764,7 @@
       <c r="A46">
         <v>2010</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>8004.0673004404207</v>
       </c>
     </row>
@@ -769,7 +772,7 @@
       <c r="A47">
         <v>2011</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>8410.3433950717354</v>
       </c>
     </row>
@@ -777,7 +780,7 @@
       <c r="A48">
         <v>2012</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>8655.3129883607235</v>
       </c>
     </row>
@@ -785,7 +788,7 @@
       <c r="A49">
         <v>2013</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>8777.3932641785595</v>
       </c>
     </row>
@@ -793,7 +796,7 @@
       <c r="A50">
         <v>2014</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>8956.6289698045966</v>
       </c>
     </row>
@@ -801,7 +804,7 @@
       <c r="A51">
         <v>2015</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>9141.3989500003827</v>
       </c>
     </row>
@@ -809,7 +812,7 @@
       <c r="A52">
         <v>2016</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>9002.8698516838904</v>
       </c>
     </row>
@@ -817,7 +820,7 @@
       <c r="A53">
         <v>2017</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>9037.0494000139734</v>
       </c>
     </row>

</xml_diff>